<commit_message>
🔥 Reupload projektu po naprawie błędu drzewa
</commit_message>
<xml_diff>
--- a/app/static/exports/prognoza_15_05.xlsx
+++ b/app/static/exports/prognoza_15_05.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prognoza" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,678 +436,514 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Godzina</t>
+          <t>Hour</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fixing I</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Fixing II</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Cena</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Hour</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Predicted Fixing I - Kurs</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Predicted Fixing II - Kurs</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Actual Fixing I - Kurs</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Actual Fixing II - Kurs</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Fixing I % Difference</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Fixing II % Difference</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>394.46</v>
+        <v>393.52</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>386.66</v>
       </c>
       <c r="D2" t="n">
-        <v>394.46</v>
+        <v>393.52</v>
       </c>
       <c r="E2" t="n">
-        <v>394.46</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+        <v>393.52</v>
+      </c>
+      <c r="F2" t="n">
+        <v>386.66</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>394.18</v>
+        <v>389.5</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>386.81</v>
       </c>
       <c r="D3" t="n">
-        <v>394.18</v>
+        <v>389.5</v>
       </c>
       <c r="E3" t="n">
-        <v>394.18</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+        <v>389.5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>386.81</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>393.58</v>
+        <v>389.28</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>386.82</v>
       </c>
       <c r="D4" t="n">
-        <v>393.58</v>
+        <v>389.28</v>
       </c>
       <c r="E4" t="n">
-        <v>393.58</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+        <v>389.28</v>
+      </c>
+      <c r="F4" t="n">
+        <v>386.82</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>393.77</v>
+        <v>388.79</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>386.79</v>
       </c>
       <c r="D5" t="n">
-        <v>393.77</v>
+        <v>388.79</v>
       </c>
       <c r="E5" t="n">
-        <v>393.77</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+        <v>388.79</v>
+      </c>
+      <c r="F5" t="n">
+        <v>386.79</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>393.72</v>
+        <v>389.86</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>395.33</v>
       </c>
       <c r="D6" t="n">
-        <v>393.72</v>
+        <v>389.86</v>
       </c>
       <c r="E6" t="n">
-        <v>393.72</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+        <v>389.86</v>
+      </c>
+      <c r="F6" t="n">
+        <v>395.33</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>390.57</v>
+        <v>394.32</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>390.67</v>
       </c>
       <c r="D7" t="n">
-        <v>390.57</v>
+        <v>394.32</v>
       </c>
       <c r="E7" t="n">
-        <v>390.57</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+        <v>394.32</v>
+      </c>
+      <c r="F7" t="n">
+        <v>390.67</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>460.8</v>
+        <v>453.55</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>405.82</v>
       </c>
       <c r="D8" t="n">
-        <v>460.8</v>
+        <v>453.55</v>
       </c>
       <c r="E8" t="n">
-        <v>460.8</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+        <v>453.55</v>
+      </c>
+      <c r="F8" t="n">
+        <v>405.82</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>447.54</v>
+        <v>427.9</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>473.57</v>
       </c>
       <c r="D9" t="n">
-        <v>447.54</v>
+        <v>427.9</v>
       </c>
       <c r="E9" t="n">
-        <v>447.54</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+        <v>427.9</v>
+      </c>
+      <c r="F9" t="n">
+        <v>473.57</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>410.52</v>
+        <v>425.4</v>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>431.17</v>
       </c>
       <c r="D10" t="n">
-        <v>410.52</v>
+        <v>425.4</v>
       </c>
       <c r="E10" t="n">
-        <v>410.52</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+        <v>425.4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>431.17</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>393.59</v>
+        <v>332.79</v>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>349.74</v>
       </c>
       <c r="D11" t="n">
-        <v>393.59</v>
+        <v>332.79</v>
       </c>
       <c r="E11" t="n">
-        <v>393.59</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+        <v>332.79</v>
+      </c>
+      <c r="F11" t="n">
+        <v>349.74</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>381.97</v>
+        <v>273.59</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>250.18</v>
       </c>
       <c r="D12" t="n">
-        <v>381.97</v>
+        <v>273.59</v>
       </c>
       <c r="E12" t="n">
-        <v>381.97</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+        <v>273.59</v>
+      </c>
+      <c r="F12" t="n">
+        <v>250.18</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>380.09</v>
+        <v>268.83</v>
       </c>
       <c r="C13" t="n">
-        <v>11</v>
+        <v>226.08</v>
       </c>
       <c r="D13" t="n">
-        <v>380.09</v>
+        <v>268.83</v>
       </c>
       <c r="E13" t="n">
-        <v>380.09</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+        <v>268.83</v>
+      </c>
+      <c r="F13" t="n">
+        <v>226.08</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>380.46</v>
+        <v>255.48</v>
       </c>
       <c r="C14" t="n">
-        <v>12</v>
+        <v>232.89</v>
       </c>
       <c r="D14" t="n">
-        <v>380.46</v>
+        <v>255.48</v>
       </c>
       <c r="E14" t="n">
-        <v>380.46</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+        <v>255.48</v>
+      </c>
+      <c r="F14" t="n">
+        <v>232.89</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>395.24</v>
+        <v>263.35</v>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>255.15</v>
       </c>
       <c r="D15" t="n">
-        <v>395.24</v>
+        <v>263.35</v>
       </c>
       <c r="E15" t="n">
-        <v>395.24</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+        <v>263.35</v>
+      </c>
+      <c r="F15" t="n">
+        <v>255.15</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>396.25</v>
+        <v>279.98</v>
       </c>
       <c r="C16" t="n">
-        <v>14</v>
+        <v>265.19</v>
       </c>
       <c r="D16" t="n">
-        <v>396.25</v>
+        <v>279.98</v>
       </c>
       <c r="E16" t="n">
-        <v>396.25</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+        <v>279.98</v>
+      </c>
+      <c r="F16" t="n">
+        <v>265.19</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>419.92</v>
+        <v>322.16</v>
       </c>
       <c r="C17" t="n">
-        <v>15</v>
+        <v>311.79</v>
       </c>
       <c r="D17" t="n">
-        <v>419.92</v>
+        <v>322.16</v>
       </c>
       <c r="E17" t="n">
-        <v>419.92</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+        <v>322.16</v>
+      </c>
+      <c r="F17" t="n">
+        <v>311.79</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>406.38</v>
+        <v>152.75</v>
       </c>
       <c r="C18" t="n">
-        <v>16</v>
+        <v>156.68</v>
       </c>
       <c r="D18" t="n">
-        <v>406.38</v>
+        <v>152.75</v>
       </c>
       <c r="E18" t="n">
-        <v>406.38</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+        <v>152.75</v>
+      </c>
+      <c r="F18" t="n">
+        <v>156.68</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>405.55</v>
+        <v>409.93</v>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>390.98</v>
       </c>
       <c r="D19" t="n">
-        <v>405.55</v>
+        <v>409.93</v>
       </c>
       <c r="E19" t="n">
-        <v>405.55</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+        <v>409.93</v>
+      </c>
+      <c r="F19" t="n">
+        <v>390.98</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>457.09</v>
+        <v>465.91</v>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>464.34</v>
       </c>
       <c r="D20" t="n">
-        <v>457.09</v>
+        <v>465.91</v>
       </c>
       <c r="E20" t="n">
-        <v>457.09</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+        <v>465.91</v>
+      </c>
+      <c r="F20" t="n">
+        <v>464.34</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>574.3</v>
+        <v>562.7</v>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>550.62</v>
       </c>
       <c r="D21" t="n">
-        <v>574.3</v>
+        <v>562.7</v>
       </c>
       <c r="E21" t="n">
-        <v>574.3</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+        <v>562.7</v>
+      </c>
+      <c r="F21" t="n">
+        <v>550.62</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>624.67</v>
+        <v>599.05</v>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>582.3099999999999</v>
       </c>
       <c r="D22" t="n">
-        <v>624.67</v>
+        <v>599.05</v>
       </c>
       <c r="E22" t="n">
-        <v>624.67</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+        <v>599.05</v>
+      </c>
+      <c r="F22" t="n">
+        <v>582.3099999999999</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>567.75</v>
+        <v>517.5599999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>21</v>
+        <v>512.0599999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>567.75</v>
+        <v>517.5599999999999</v>
       </c>
       <c r="E23" t="n">
-        <v>567.75</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+        <v>517.5599999999999</v>
+      </c>
+      <c r="F23" t="n">
+        <v>512.0599999999999</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>460.26</v>
+        <v>455.22</v>
       </c>
       <c r="C24" t="n">
-        <v>22</v>
+        <v>439.26</v>
       </c>
       <c r="D24" t="n">
-        <v>460.26</v>
+        <v>455.22</v>
       </c>
       <c r="E24" t="n">
-        <v>460.26</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+        <v>455.22</v>
+      </c>
+      <c r="F24" t="n">
+        <v>439.26</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>408.53</v>
+        <v>419.87</v>
       </c>
       <c r="C25" t="n">
-        <v>23</v>
+        <v>377.03</v>
       </c>
       <c r="D25" t="n">
-        <v>408.53</v>
+        <v>419.87</v>
       </c>
       <c r="E25" t="n">
-        <v>408.53</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+        <v>419.87</v>
+      </c>
+      <c r="F25" t="n">
+        <v>377.03</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>